<commit_message>
feat: handling iops and disk utilization
</commit_message>
<xml_diff>
--- a/gcp_vm_inventory_mpa.xlsx
+++ b/gcp_vm_inventory_mpa.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -526,7 +526,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>mariadb-2-vm</t>
+          <t>instance-20240725-115904</t>
         </is>
       </c>
       <c r="B2" t="b">
@@ -539,10 +539,14 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>mariadb-2-vm</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr"/>
+          <t>instance-20240725-115904</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>X86_64</t>
+        </is>
+      </c>
       <c r="G2" t="n">
         <v>2</v>
       </c>
@@ -553,27 +557,80 @@
         <v>1</v>
       </c>
       <c r="J2" t="n">
-        <v>22.49537404952985</v>
+        <v/>
       </c>
       <c r="K2" t="n">
-        <v>10.29494970353895</v>
+        <v/>
       </c>
       <c r="L2" t="n">
+        <v>1</v>
+      </c>
+      <c r="M2" t="n">
+        <v/>
+      </c>
+      <c r="N2" t="n">
+        <v/>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>Production</t>
+        </is>
+      </c>
+      <c r="Q2" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>mariadb-2-vm</t>
+        </is>
+      </c>
+      <c r="B3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Google Compute Engine</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>mariadb-2-vm</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="G3" t="n">
+        <v>2</v>
+      </c>
+      <c r="H3" t="n">
+        <v>1</v>
+      </c>
+      <c r="I3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J3" t="n">
+        <v>21.49573552293964</v>
+      </c>
+      <c r="K3" t="n">
+        <v>10.28462705365895</v>
+      </c>
+      <c r="L3" t="n">
         <v>4</v>
       </c>
-      <c r="M2" t="n">
-        <v>0.6984972917295282</v>
-      </c>
-      <c r="N2" t="n">
-        <v>0.6693799370912564</v>
-      </c>
-      <c r="P2" t="inlineStr">
+      <c r="M3" t="n">
+        <v>0.6997745921401075</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0.6694750599138971</v>
+      </c>
+      <c r="P3" t="inlineStr">
         <is>
           <t>Production</t>
         </is>
       </c>
-      <c r="Q2" t="n">
-        <v>30</v>
+      <c r="Q3" t="n">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>